<commit_message>
reporte de conexiones por usuario listo
</commit_message>
<xml_diff>
--- a/docs/formatos/conexionesUsuarios.xlsx
+++ b/docs/formatos/conexionesUsuarios.xlsx
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +110,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,12 +149,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -155,7 +182,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -171,9 +197,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -189,8 +220,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -473,28 +514,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.140625" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" customWidth="1"/>
+    <col min="13" max="13" width="34" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
     <col min="15" max="15" width="60.7109375" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="8.7109375" customWidth="1"/>
@@ -502,142 +543,158 @@
     <col min="19" max="19" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+    <row r="1" spans="1:19" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G10" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajuste formato de reportes conexionesUsuario
</commit_message>
<xml_diff>
--- a/docs/formatos/conexionesUsuarios.xlsx
+++ b/docs/formatos/conexionesUsuarios.xlsx
@@ -57,10 +57,10 @@
     <t>Campo4</t>
   </si>
   <si>
-    <t>Tiempo promedio de conexiones</t>
-  </si>
-  <si>
     <t>Cantidad de conexiones</t>
+  </si>
+  <si>
+    <t>Tiempo de conexion acumulado</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="69" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="H1" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="69" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,10 +661,10 @@
         <v>11</v>
       </c>
       <c r="M4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>

</xml_diff>

<commit_message>
Agregando hora de registro a reporte: conexiones por participante
</commit_message>
<xml_diff>
--- a/docs/formatos/conexionesUsuarios.xlsx
+++ b/docs/formatos/conexionesUsuarios.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22609"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36E341B9-E4B9-49A1-AABE-F63874847EF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Código</t>
   </si>
@@ -31,9 +42,15 @@
     <t>Fecha de Registro</t>
   </si>
   <si>
+    <t>Hora de Registro</t>
+  </si>
+  <si>
     <t>Correo</t>
   </si>
   <si>
+    <t>Acceso</t>
+  </si>
+  <si>
     <t>País</t>
   </si>
   <si>
@@ -52,20 +69,17 @@
     <t>Campo4</t>
   </si>
   <si>
+    <t>Tiempo de conexion acumulado</t>
+  </si>
+  <si>
     <t>Cantidad de conexiones</t>
-  </si>
-  <si>
-    <t>Tiempo de conexion acumulado</t>
-  </si>
-  <si>
-    <t>Acceso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -140,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -183,11 +197,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,81 +546,88 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="69" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="69" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" customWidth="1"/>
-    <col min="13" max="13" width="34" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" customWidth="1"/>
-    <col min="15" max="15" width="60.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="4" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="13" max="13" width="30.140625" customWidth="1"/>
+    <col min="14" max="14" width="34" customWidth="1"/>
+    <col min="15" max="15" width="25.42578125" customWidth="1"/>
+    <col min="16" max="16" width="60.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-    </row>
-    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+    </row>
+    <row r="2" spans="1:20" ht="20.25" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+    </row>
+    <row r="3" spans="1:20">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -616,14 +640,15 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -642,60 +667,64 @@
       <c r="F4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="H4" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I4" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="24.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="11"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="6"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="8"/>
+      <c r="R5" s="7"/>
       <c r="S5" s="8"/>
-    </row>
-    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" ht="20.25" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -710,8 +739,9 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" ht="22.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -726,21 +756,22 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G10" s="9"/>
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="H10" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>